<commit_message>
Finalization of the Reports through GA4 and Chartbeat
</commit_message>
<xml_diff>
--- a/AnalyticsReport.xlsx
+++ b/AnalyticsReport.xlsx
@@ -397,18 +397,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="25.83203125" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" customWidth="1"/>
+    <col min="3" max="3" width="25.83203125" customWidth="1"/>
     <col min="4" max="4" width="15.83203125" customWidth="1"/>
-    <col min="5" max="5" width="15.83203125" customWidth="1"/>
-    <col min="6" max="6" width="20.83203125" customWidth="1"/>
-    <col min="7" max="7" width="35.83203125" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" customWidth="1"/>
+    <col min="8" max="8" width="20.83203125" customWidth="1"/>
+    <col min="9" max="9" width="35.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -436,18 +438,27 @@
         <v>Site</v>
       </c>
       <c r="B2" t="str">
+        <v>Adsense Revenue</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Total users (chartbeat)</v>
+      </c>
+      <c r="D2" t="str">
+        <v>Views (chartbeat)</v>
+      </c>
+      <c r="E2" t="str">
         <v>Total Users (GA4)</v>
       </c>
-      <c r="C2" t="str">
+      <c r="F2" t="str">
         <v>Views (GA4)</v>
       </c>
-      <c r="D2" t="str">
+      <c r="G2" t="str">
         <v>Views per user</v>
       </c>
-      <c r="E2" t="str">
+      <c r="H2" t="str">
         <v>Engagement rate</v>
       </c>
-      <c r="F2" t="str">
+      <c r="I2" t="str">
         <v>Average engagement time</v>
       </c>
     </row>
@@ -456,18 +467,27 @@
         <v>www.athensmagazine.gr</v>
       </c>
       <c r="B3" t="str">
+        <v/>
+      </c>
+      <c r="C3" t="str">
+        <v>153.619</v>
+      </c>
+      <c r="D3" t="str">
+        <v>88.845</v>
+      </c>
+      <c r="E3" t="str">
         <v>78.657</v>
       </c>
-      <c r="C3" t="str">
+      <c r="F3" t="str">
         <v>134.087</v>
       </c>
-      <c r="D3" t="str">
+      <c r="G3" t="str">
         <v>2.17</v>
       </c>
-      <c r="E3" t="str">
+      <c r="H3" t="str">
         <v>57.00%</v>
       </c>
-      <c r="F3" t="str">
+      <c r="I3" t="str">
         <v>1m 06s</v>
       </c>
     </row>
@@ -476,18 +496,27 @@
         <v>www.youweekly.gr</v>
       </c>
       <c r="B4" t="str">
+        <v/>
+      </c>
+      <c r="C4" t="str">
+        <v>136.241</v>
+      </c>
+      <c r="D4" t="str">
+        <v>71.161</v>
+      </c>
+      <c r="E4" t="str">
         <v>64.573</v>
       </c>
-      <c r="C4" t="str">
+      <c r="F4" t="str">
         <v>133.175</v>
       </c>
-      <c r="D4" t="str">
+      <c r="G4" t="str">
         <v>2.43</v>
       </c>
-      <c r="E4" t="str">
+      <c r="H4" t="str">
         <v>65.00%</v>
       </c>
-      <c r="F4" t="str">
+      <c r="I4" t="str">
         <v>1m 28s</v>
       </c>
     </row>
@@ -496,24 +525,33 @@
         <v>www.travelstyle.gr</v>
       </c>
       <c r="B5" t="str">
+        <v/>
+      </c>
+      <c r="C5" t="str">
+        <v>6.581</v>
+      </c>
+      <c r="D5" t="str">
+        <v>4.745</v>
+      </c>
+      <c r="E5" t="str">
         <v>2.227</v>
       </c>
-      <c r="C5" t="str">
+      <c r="F5" t="str">
         <v>3.249</v>
       </c>
-      <c r="D5" t="str">
+      <c r="G5" t="str">
         <v>1.52</v>
       </c>
-      <c r="E5" t="str">
+      <c r="H5" t="str">
         <v>61.00%</v>
       </c>
-      <c r="F5" t="str">
+      <c r="I5" t="str">
         <v>1m 08s</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>